<commit_message>
service ImportBasePrixRef() et tests
</commit_message>
<xml_diff>
--- a/templates & procedures/templateBasePrix.xlsx
+++ b/templates & procedures/templateBasePrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentinmarc/Documents/ETIC-git/Etude BRP/templates &amp; procedures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisrob/Documents/ETIC/Etude_BRP/templates &amp; procedures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA3F86E-13B8-6B43-A65E-576BFF4AAE21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709EFFF9-C357-D042-B8FD-655FCB2A927A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{9FBCDC7A-2121-CC48-B5E9-95AF4E436D87}"/>
+    <workbookView xWindow="160" yWindow="700" windowWidth="28800" windowHeight="15800" xr2:uid="{9FBCDC7A-2121-CC48-B5E9-95AF4E436D87}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>unite</t>
   </si>
@@ -42,15 +42,6 @@
     <t>anneeRef</t>
   </si>
   <si>
-    <t>Ouvrage (/)</t>
-  </si>
-  <si>
-    <t>Prestation (/)</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>0.98</t>
   </si>
   <si>
@@ -94,6 +85,12 @@
   </si>
   <si>
     <t>04_AAA_01_01_01_02</t>
+  </si>
+  <si>
+    <t>Ouvrage/Prestation</t>
+  </si>
+  <si>
+    <t>NbPrixRef</t>
   </si>
 </sst>
 </file>
@@ -477,29 +474,29 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -508,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -522,19 +519,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -543,7 +540,7 @@
         <v>100</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1">
         <v>200</v>
@@ -554,19 +551,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -575,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1">
         <v>500</v>
@@ -586,16 +583,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>

</xml_diff>